<commit_message>
practice data driven test
</commit_message>
<xml_diff>
--- a/JavaSeleniumPractice/test-data/dynamicData.xlsx
+++ b/JavaSeleniumPractice/test-data/dynamicData.xlsx
@@ -7,41 +7,39 @@
   </bookViews>
   <sheets>
     <sheet name="DyanamicData" r:id="rId3" sheetId="1"/>
+    <sheet name="DyanamicData2" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>"Name"</t>
+    <t>Shivam</t>
   </si>
   <si>
-    <t>"Surname"</t>
+    <t>Komawar</t>
   </si>
   <si>
-    <t>"Shivam"</t>
+    <t>Shubham</t>
   </si>
   <si>
-    <t>"Komawar"</t>
+    <t>Uttarwar</t>
   </si>
   <si>
-    <t>"pratik"</t>
+    <t>Aditya</t>
   </si>
   <si>
-    <t>"motipwar"</t>
+    <t>uttarwar</t>
   </si>
   <si>
-    <t>"Shubham"</t>
+    <t>Java</t>
   </si>
   <si>
-    <t>"Uttarwar"</t>
+    <t>Selenium</t>
   </si>
   <si>
-    <t>Aditya"</t>
-  </si>
-  <si>
-    <t>"Lingawar"</t>
+    <t>python</t>
   </si>
 </sst>
 </file>
@@ -86,7 +84,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -99,41 +97,49 @@
       <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
         <v>2</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>6</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s" s="0">
         <v>8</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>